<commit_message>
Update data and scripts for Zambia model
</commit_message>
<xml_diff>
--- a/nest/message_ix_models/data/leap_re_nest/OnSSET_cost_paramters.xlsx
+++ b/nest/message_ix_models/data/leap_re_nest/OnSSET_cost_paramters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinca\Documents\Github\message_data_LEAPRE\data\projects\leap_re_nest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B606FE-EB37-42EF-B391-9421CA9457D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8510F177-0D17-4EFB-AC87-7E03016390A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OnSSET_cost_paramters" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="139">
   <si>
     <t>Variable</t>
   </si>
@@ -440,6 +440,15 @@
   </si>
   <si>
     <t>sa_diesel</t>
+  </si>
+  <si>
+    <t>mg_pv_hybrid</t>
+  </si>
+  <si>
+    <t>mg_wind_hybrid</t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -1282,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,13 +2022,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2078,6 +2090,31 @@
         <v>938</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B9)</f>
+        <v>2737.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>